<commit_message>
mode 1 release 1 analysis done
</commit_message>
<xml_diff>
--- a/Human_Evaluation/Helpers/mode_1_release_1_test_samples_manual_evaluation.xlsx
+++ b/Human_Evaluation/Helpers/mode_1_release_1_test_samples_manual_evaluation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tkang/Documents/research/nlp_followupqg/Human_Evaluation/Helpers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F284C5B7-6ED8-0444-95A1-EAA8B32A26C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16771A3E-21F6-914D-98CB-ACB13CB8E9D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18140" yWindow="-28300" windowWidth="34400" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -464,7 +464,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="192" zoomScaleNormal="192" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -657,7 +657,7 @@
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Zhe's manual labeling added (currently just mode 1))
</commit_message>
<xml_diff>
--- a/Human_Evaluation/Helpers/mode_1_release_1_test_samples_manual_evaluation.xlsx
+++ b/Human_Evaluation/Helpers/mode_1_release_1_test_samples_manual_evaluation.xlsx
@@ -5,22 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tkang/Documents/research/nlp_followupqg/Human_Evaluation/Helpers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhe/Documents/GitHub/nlp_followupqg/Human_Evaluation/Helpers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16771A3E-21F6-914D-98CB-ACB13CB8E9D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A62050-9901-FD4F-AD30-1477DA0BF6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="26">
   <si>
     <t>group</t>
   </si>
@@ -463,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="192" zoomScaleNormal="192" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView zoomScale="192" zoomScaleNormal="192" workbookViewId="0">
+      <selection sqref="A1:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -666,4 +667,206 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADFAE41D-0FB6-AC4F-8352-FD31BC706A75}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>